<commit_message>
finally managed to find the bug
</commit_message>
<xml_diff>
--- a/datacombined dataloggerMSLmi70.xlsx.xlsx
+++ b/datacombined dataloggerMSLmi70.xlsx.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BP44"/>
+  <dimension ref="A1:BO44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -720,55 +720,50 @@
       </c>
       <c r="BF1" s="1" t="inlineStr">
         <is>
-          <t>datetime before shift</t>
-        </is>
-      </c>
-      <c r="BG1" s="1" t="inlineStr">
-        <is>
           <t>mean no</t>
         </is>
       </c>
-      <c r="BH1" s="1" t="inlineStr">
+      <c r="BG1" s="1" t="inlineStr">
         <is>
           <t>std no</t>
         </is>
       </c>
-      <c r="BI1" s="1" t="inlineStr">
+      <c r="BH1" s="1" t="inlineStr">
         <is>
           <t>DUT datetime</t>
         </is>
       </c>
-      <c r="BJ1" s="1" t="inlineStr">
+      <c r="BI1" s="1" t="inlineStr">
         <is>
           <t>mean RH, %</t>
         </is>
       </c>
-      <c r="BK1" s="1" t="inlineStr">
+      <c r="BJ1" s="1" t="inlineStr">
         <is>
           <t>std RH, %</t>
         </is>
       </c>
-      <c r="BL1" s="1" t="inlineStr">
+      <c r="BK1" s="1" t="inlineStr">
         <is>
           <t>mean T</t>
         </is>
       </c>
-      <c r="BM1" s="1" t="inlineStr">
+      <c r="BL1" s="1" t="inlineStr">
         <is>
           <t>std T</t>
         </is>
       </c>
-      <c r="BN1" s="1" t="inlineStr">
+      <c r="BM1" s="1" t="inlineStr">
         <is>
           <t>mean Td/f</t>
         </is>
       </c>
-      <c r="BO1" s="1" t="inlineStr">
+      <c r="BN1" s="1" t="inlineStr">
         <is>
           <t>std Td/f</t>
         </is>
       </c>
-      <c r="BP1" s="1" t="inlineStr">
+      <c r="BO1" s="1" t="inlineStr">
         <is>
           <t>datetime shifted</t>
         </is>
@@ -782,7 +777,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>44629.72873842593</v>
+        <v>44629.73568287037</v>
       </c>
       <c r="D2" t="n">
         <v>240.042469784617</v>
@@ -946,38 +941,35 @@
       <c r="BE2" t="n">
         <v>10</v>
       </c>
-      <c r="BF2" s="2" t="n">
+      <c r="BF2" t="n">
+        <v>285.5</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH2" s="2" t="n">
+        <v>44629.73611111111</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>10.362</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>0.009189365834726898</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>5.049999999999999</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>-21.345</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>0.009718253158076985</v>
+      </c>
+      <c r="BO2" s="2" t="n">
         <v>44629.73568287037</v>
-      </c>
-      <c r="BG2" t="n">
-        <v>335.5</v>
-      </c>
-      <c r="BH2" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI2" s="2" t="n">
-        <v>44629.76701388889</v>
-      </c>
-      <c r="BJ2" t="n">
-        <v>31.906</v>
-      </c>
-      <c r="BK2" t="n">
-        <v>0.006992058987802655</v>
-      </c>
-      <c r="BL2" t="n">
-        <v>5.06</v>
-      </c>
-      <c r="BM2" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN2" t="n">
-        <v>-9.181000000000001</v>
-      </c>
-      <c r="BO2" t="n">
-        <v>0.003162277660167868</v>
-      </c>
-      <c r="BP2" s="2" t="n">
-        <v>44629.73221064815</v>
       </c>
     </row>
     <row r="3">
@@ -988,7 +980,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>44629.76385416667</v>
+        <v>44629.77079861111</v>
       </c>
       <c r="D3" t="n">
         <v>290.609363105148</v>
@@ -1152,38 +1144,35 @@
       <c r="BE3" t="n">
         <v>10</v>
       </c>
-      <c r="BF3" s="2" t="n">
+      <c r="BF3" t="n">
+        <v>335.5</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH3" s="2" t="n">
+        <v>44629.77083333334</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>31.906</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>0.006992058987802655</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>5.06</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>-9.181000000000001</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>0.003162277660167868</v>
+      </c>
+      <c r="BO3" s="2" t="n">
         <v>44629.77079861111</v>
-      </c>
-      <c r="BG3" t="n">
-        <v>387.5</v>
-      </c>
-      <c r="BH3" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI3" s="2" t="n">
-        <v>44629.803125</v>
-      </c>
-      <c r="BJ3" t="n">
-        <v>52.789</v>
-      </c>
-      <c r="BK3" t="n">
-        <v>0.05216427044549821</v>
-      </c>
-      <c r="BL3" t="n">
-        <v>5.06</v>
-      </c>
-      <c r="BM3" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN3" t="n">
-        <v>-3.348</v>
-      </c>
-      <c r="BO3" t="n">
-        <v>0.01316561177208773</v>
-      </c>
-      <c r="BP3" s="2" t="n">
-        <v>44629.76732638889</v>
       </c>
     </row>
     <row r="4">
@@ -1194,7 +1183,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>44629.79940972223</v>
+        <v>44629.80635416666</v>
       </c>
       <c r="D4" t="n">
         <v>341.799214676022</v>
@@ -1358,38 +1347,35 @@
       <c r="BE4" t="n">
         <v>10</v>
       </c>
-      <c r="BF4" s="2" t="n">
+      <c r="BF4" t="n">
+        <v>387.5</v>
+      </c>
+      <c r="BG4" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH4" s="2" t="n">
+        <v>44629.80694444444</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>52.789</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>0.05216427044549821</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>5.06</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>-3.348</v>
+      </c>
+      <c r="BN4" t="n">
+        <v>0.01316561177208773</v>
+      </c>
+      <c r="BO4" s="2" t="n">
         <v>44629.80635416666</v>
-      </c>
-      <c r="BG4" t="n">
-        <v>438.5</v>
-      </c>
-      <c r="BH4" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI4" s="2" t="n">
-        <v>44629.83854166666</v>
-      </c>
-      <c r="BJ4" t="n">
-        <v>74.01899999999999</v>
-      </c>
-      <c r="BK4" t="n">
-        <v>0.01286683937707885</v>
-      </c>
-      <c r="BL4" t="n">
-        <v>5.062</v>
-      </c>
-      <c r="BM4" t="n">
-        <v>0.004216370213557746</v>
-      </c>
-      <c r="BN4" t="n">
-        <v>0.827</v>
-      </c>
-      <c r="BO4" t="n">
-        <v>0.004830458915396482</v>
-      </c>
-      <c r="BP4" s="2" t="n">
-        <v>44629.80288194444</v>
       </c>
     </row>
     <row r="5">
@@ -1400,7 +1386,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>44629.8350462963</v>
+        <v>44629.84199074074</v>
       </c>
       <c r="D5" t="n">
         <v>393.119193006306</v>
@@ -1564,38 +1550,35 @@
       <c r="BE5" t="n">
         <v>10</v>
       </c>
-      <c r="BF5" s="2" t="n">
+      <c r="BF5" t="n">
+        <v>438.5</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH5" s="2" t="n">
+        <v>44629.84236111111</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>74.01899999999999</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>0.01286683937707885</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>5.062</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>0.004216370213557746</v>
+      </c>
+      <c r="BM5" t="n">
+        <v>0.827</v>
+      </c>
+      <c r="BN5" t="n">
+        <v>0.004830458915396482</v>
+      </c>
+      <c r="BO5" s="2" t="n">
         <v>44629.84199074074</v>
-      </c>
-      <c r="BG5" t="n">
-        <v>489.5</v>
-      </c>
-      <c r="BH5" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI5" s="2" t="n">
-        <v>44629.87395833333</v>
-      </c>
-      <c r="BJ5" t="n">
-        <v>94.31399999999996</v>
-      </c>
-      <c r="BK5" t="n">
-        <v>0.008432740427116536</v>
-      </c>
-      <c r="BL5" t="n">
-        <v>5.087999999999999</v>
-      </c>
-      <c r="BM5" t="n">
-        <v>0.004216370213557779</v>
-      </c>
-      <c r="BN5" t="n">
-        <v>4.25</v>
-      </c>
-      <c r="BO5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BP5" s="2" t="n">
-        <v>44629.83851851852</v>
       </c>
     </row>
     <row r="6">
@@ -1606,7 +1589,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>44629.87075231481</v>
+        <v>44629.87769675926</v>
       </c>
       <c r="D6" t="n">
         <v>444.537089899182</v>
@@ -1770,38 +1753,35 @@
       <c r="BE6" t="n">
         <v>10</v>
       </c>
-      <c r="BF6" s="2" t="n">
+      <c r="BF6" t="n">
+        <v>489.5</v>
+      </c>
+      <c r="BG6" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH6" s="2" t="n">
+        <v>44629.87777777778</v>
+      </c>
+      <c r="BI6" t="n">
+        <v>94.31399999999996</v>
+      </c>
+      <c r="BJ6" t="n">
+        <v>0.008432740427116536</v>
+      </c>
+      <c r="BK6" t="n">
+        <v>5.087999999999999</v>
+      </c>
+      <c r="BL6" t="n">
+        <v>0.004216370213557779</v>
+      </c>
+      <c r="BM6" t="n">
+        <v>4.25</v>
+      </c>
+      <c r="BN6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO6" s="2" t="n">
         <v>44629.87769675926</v>
-      </c>
-      <c r="BG6" t="n">
-        <v>541.5</v>
-      </c>
-      <c r="BH6" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI6" s="2" t="n">
-        <v>44629.91006944444</v>
-      </c>
-      <c r="BJ6" t="n">
-        <v>74.303</v>
-      </c>
-      <c r="BK6" t="n">
-        <v>0.05143496432929512</v>
-      </c>
-      <c r="BL6" t="n">
-        <v>5.037999999999999</v>
-      </c>
-      <c r="BM6" t="n">
-        <v>0.00421637021355761</v>
-      </c>
-      <c r="BN6" t="n">
-        <v>0.853</v>
-      </c>
-      <c r="BO6" t="n">
-        <v>0.008232726023485624</v>
-      </c>
-      <c r="BP6" s="2" t="n">
-        <v>44629.87422453704</v>
       </c>
     </row>
     <row r="7">
@@ -1812,7 +1792,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>44629.90653935185</v>
+        <v>44629.9134837963</v>
       </c>
       <c r="D7" t="n">
         <v>496.077166128903</v>
@@ -1976,38 +1956,35 @@
       <c r="BE7" t="n">
         <v>10</v>
       </c>
-      <c r="BF7" s="2" t="n">
+      <c r="BF7" t="n">
+        <v>541.5</v>
+      </c>
+      <c r="BG7" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH7" s="2" t="n">
+        <v>44629.91388888889</v>
+      </c>
+      <c r="BI7" t="n">
+        <v>74.303</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>0.05143496432929512</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>5.037999999999999</v>
+      </c>
+      <c r="BL7" t="n">
+        <v>0.00421637021355761</v>
+      </c>
+      <c r="BM7" t="n">
+        <v>0.853</v>
+      </c>
+      <c r="BN7" t="n">
+        <v>0.008232726023485624</v>
+      </c>
+      <c r="BO7" s="2" t="n">
         <v>44629.9134837963</v>
-      </c>
-      <c r="BG7" t="n">
-        <v>591.5</v>
-      </c>
-      <c r="BH7" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI7" s="2" t="n">
-        <v>44629.94479166667</v>
-      </c>
-      <c r="BJ7" t="n">
-        <v>53.11900000000001</v>
-      </c>
-      <c r="BK7" t="n">
-        <v>0.007378647873729009</v>
-      </c>
-      <c r="BL7" t="n">
-        <v>5.04</v>
-      </c>
-      <c r="BM7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN7" t="n">
-        <v>-3.29</v>
-      </c>
-      <c r="BO7" t="n">
-        <v>0</v>
-      </c>
-      <c r="BP7" s="2" t="n">
-        <v>44629.91001157407</v>
       </c>
     </row>
     <row r="8">
@@ -2018,7 +1995,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>44629.94127314815</v>
+        <v>44629.9482175926</v>
       </c>
       <c r="D8" t="n">
         <v>546.093313217163</v>
@@ -2182,38 +2159,35 @@
       <c r="BE8" t="n">
         <v>10</v>
       </c>
-      <c r="BF8" s="2" t="n">
+      <c r="BF8" t="n">
+        <v>591.5</v>
+      </c>
+      <c r="BG8" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH8" s="2" t="n">
+        <v>44629.94861111111</v>
+      </c>
+      <c r="BI8" t="n">
+        <v>53.11900000000001</v>
+      </c>
+      <c r="BJ8" t="n">
+        <v>0.007378647873729009</v>
+      </c>
+      <c r="BK8" t="n">
+        <v>5.04</v>
+      </c>
+      <c r="BL8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM8" t="n">
+        <v>-3.29</v>
+      </c>
+      <c r="BN8" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO8" s="2" t="n">
         <v>44629.9482175926</v>
-      </c>
-      <c r="BG8" t="n">
-        <v>642.5</v>
-      </c>
-      <c r="BH8" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI8" s="2" t="n">
-        <v>44629.98020833333</v>
-      </c>
-      <c r="BJ8" t="n">
-        <v>32.186</v>
-      </c>
-      <c r="BK8" t="n">
-        <v>0.006992058987801912</v>
-      </c>
-      <c r="BL8" t="n">
-        <v>5.04</v>
-      </c>
-      <c r="BM8" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN8" t="n">
-        <v>-9.096</v>
-      </c>
-      <c r="BO8" t="n">
-        <v>0.005163977794943253</v>
-      </c>
-      <c r="BP8" s="2" t="n">
-        <v>44629.94474537037</v>
       </c>
     </row>
     <row r="9">
@@ -2224,7 +2198,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>44629.97693287037</v>
+        <v>44629.98387731481</v>
       </c>
       <c r="D9" t="n">
         <v>597.4387266412371</v>
@@ -2388,38 +2362,35 @@
       <c r="BE9" t="n">
         <v>10</v>
       </c>
-      <c r="BF9" s="2" t="n">
+      <c r="BF9" t="n">
+        <v>642.5</v>
+      </c>
+      <c r="BG9" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH9" s="2" t="n">
+        <v>44629.98402777778</v>
+      </c>
+      <c r="BI9" t="n">
+        <v>32.186</v>
+      </c>
+      <c r="BJ9" t="n">
+        <v>0.006992058987801912</v>
+      </c>
+      <c r="BK9" t="n">
+        <v>5.04</v>
+      </c>
+      <c r="BL9" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM9" t="n">
+        <v>-9.096</v>
+      </c>
+      <c r="BN9" t="n">
+        <v>0.005163977794943253</v>
+      </c>
+      <c r="BO9" s="2" t="n">
         <v>44629.98387731481</v>
-      </c>
-      <c r="BG9" t="n">
-        <v>694.5</v>
-      </c>
-      <c r="BH9" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI9" s="2" t="n">
-        <v>44630.01631944445</v>
-      </c>
-      <c r="BJ9" t="n">
-        <v>10.527</v>
-      </c>
-      <c r="BK9" t="n">
-        <v>0.009486832980504971</v>
-      </c>
-      <c r="BL9" t="n">
-        <v>5.04</v>
-      </c>
-      <c r="BM9" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN9" t="n">
-        <v>-21.193</v>
-      </c>
-      <c r="BO9" t="n">
-        <v>0.009486832980504635</v>
-      </c>
-      <c r="BP9" s="2" t="n">
-        <v>44629.9804050926</v>
       </c>
     </row>
     <row r="10">
@@ -2430,7 +2401,7 @@
         <v>9</v>
       </c>
       <c r="C10" s="2" t="n">
-        <v>44630.01263888889</v>
+        <v>44630.01958333333</v>
       </c>
       <c r="D10" t="n">
         <v>648.846525467932</v>
@@ -2594,38 +2565,35 @@
       <c r="BE10" t="n">
         <v>10</v>
       </c>
-      <c r="BF10" s="2" t="n">
+      <c r="BF10" t="n">
+        <v>694.5</v>
+      </c>
+      <c r="BG10" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH10" s="2" t="n">
+        <v>44630.02013888889</v>
+      </c>
+      <c r="BI10" t="n">
+        <v>10.527</v>
+      </c>
+      <c r="BJ10" t="n">
+        <v>0.009486832980504971</v>
+      </c>
+      <c r="BK10" t="n">
+        <v>5.04</v>
+      </c>
+      <c r="BL10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM10" t="n">
+        <v>-21.193</v>
+      </c>
+      <c r="BN10" t="n">
+        <v>0.009486832980504635</v>
+      </c>
+      <c r="BO10" s="2" t="n">
         <v>44630.01958333333</v>
-      </c>
-      <c r="BG10" t="n">
-        <v>874.5</v>
-      </c>
-      <c r="BH10" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI10" s="2" t="n">
-        <v>44630.14131944445</v>
-      </c>
-      <c r="BJ10" t="n">
-        <v>10.38</v>
-      </c>
-      <c r="BK10" t="n">
-        <v>0.006666666666667008</v>
-      </c>
-      <c r="BL10" t="n">
-        <v>15.01</v>
-      </c>
-      <c r="BM10" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN10" t="n">
-        <v>-14.255</v>
-      </c>
-      <c r="BO10" t="n">
-        <v>0.007071067811865254</v>
-      </c>
-      <c r="BP10" s="2" t="n">
-        <v>44630.01611111111</v>
       </c>
     </row>
     <row r="11">
@@ -2636,7 +2604,7 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="n">
-        <v>44630.13788194444</v>
+        <v>44630.14482638889</v>
       </c>
       <c r="D11" t="n">
         <v>829.200128857046</v>
@@ -2800,38 +2768,35 @@
       <c r="BE11" t="n">
         <v>10</v>
       </c>
-      <c r="BF11" s="2" t="n">
+      <c r="BF11" t="n">
+        <v>874.5</v>
+      </c>
+      <c r="BG11" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH11" s="2" t="n">
+        <v>44630.14513888889</v>
+      </c>
+      <c r="BI11" t="n">
+        <v>10.38</v>
+      </c>
+      <c r="BJ11" t="n">
+        <v>0.006666666666667008</v>
+      </c>
+      <c r="BK11" t="n">
+        <v>15.01</v>
+      </c>
+      <c r="BL11" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM11" t="n">
+        <v>-14.255</v>
+      </c>
+      <c r="BN11" t="n">
+        <v>0.007071067811865254</v>
+      </c>
+      <c r="BO11" s="2" t="n">
         <v>44630.14482638889</v>
-      </c>
-      <c r="BG11" t="n">
-        <v>924.5</v>
-      </c>
-      <c r="BH11" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI11" s="2" t="n">
-        <v>44630.17604166667</v>
-      </c>
-      <c r="BJ11" t="n">
-        <v>31.8</v>
-      </c>
-      <c r="BK11" t="n">
-        <v>0.008164965809275393</v>
-      </c>
-      <c r="BL11" t="n">
-        <v>15.018</v>
-      </c>
-      <c r="BM11" t="n">
-        <v>0.004216370213557835</v>
-      </c>
-      <c r="BN11" t="n">
-        <v>-1.44</v>
-      </c>
-      <c r="BO11" t="n">
-        <v>0</v>
-      </c>
-      <c r="BP11" s="2" t="n">
-        <v>44630.14135416667</v>
       </c>
     </row>
     <row r="12">
@@ -2842,7 +2807,7 @@
         <v>11</v>
       </c>
       <c r="C12" s="2" t="n">
-        <v>44630.17275462963</v>
+        <v>44630.17969907408</v>
       </c>
       <c r="D12" t="n">
         <v>879.42343147099</v>
@@ -3006,38 +2971,35 @@
       <c r="BE12" t="n">
         <v>10</v>
       </c>
-      <c r="BF12" s="2" t="n">
+      <c r="BF12" t="n">
+        <v>924.5</v>
+      </c>
+      <c r="BG12" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH12" s="2" t="n">
+        <v>44630.17986111111</v>
+      </c>
+      <c r="BI12" t="n">
+        <v>31.8</v>
+      </c>
+      <c r="BJ12" t="n">
+        <v>0.008164965809275393</v>
+      </c>
+      <c r="BK12" t="n">
+        <v>15.018</v>
+      </c>
+      <c r="BL12" t="n">
+        <v>0.004216370213557835</v>
+      </c>
+      <c r="BM12" t="n">
+        <v>-1.44</v>
+      </c>
+      <c r="BN12" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO12" s="2" t="n">
         <v>44630.17969907408</v>
-      </c>
-      <c r="BG12" t="n">
-        <v>975.5</v>
-      </c>
-      <c r="BH12" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI12" s="2" t="n">
-        <v>44630.21145833333</v>
-      </c>
-      <c r="BJ12" t="n">
-        <v>52.642</v>
-      </c>
-      <c r="BK12" t="n">
-        <v>0.004216370213557572</v>
-      </c>
-      <c r="BL12" t="n">
-        <v>15.02</v>
-      </c>
-      <c r="BM12" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN12" t="n">
-        <v>5.427</v>
-      </c>
-      <c r="BO12" t="n">
-        <v>0.004830458915396457</v>
-      </c>
-      <c r="BP12" s="2" t="n">
-        <v>44630.17622685185</v>
       </c>
     </row>
     <row r="13">
@@ -3048,7 +3010,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="2" t="n">
-        <v>44630.2080324074</v>
+        <v>44630.21497685185</v>
       </c>
       <c r="D13" t="n">
         <v>930.216426521539</v>
@@ -3212,38 +3174,35 @@
       <c r="BE13" t="n">
         <v>10</v>
       </c>
-      <c r="BF13" s="2" t="n">
+      <c r="BF13" t="n">
+        <v>975.5</v>
+      </c>
+      <c r="BG13" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH13" s="2" t="n">
+        <v>44630.21527777778</v>
+      </c>
+      <c r="BI13" t="n">
+        <v>52.642</v>
+      </c>
+      <c r="BJ13" t="n">
+        <v>0.004216370213557572</v>
+      </c>
+      <c r="BK13" t="n">
+        <v>15.02</v>
+      </c>
+      <c r="BL13" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM13" t="n">
+        <v>5.427</v>
+      </c>
+      <c r="BN13" t="n">
+        <v>0.004830458915396457</v>
+      </c>
+      <c r="BO13" s="2" t="n">
         <v>44630.21497685185</v>
-      </c>
-      <c r="BG13" t="n">
-        <v>1026.5</v>
-      </c>
-      <c r="BH13" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI13" s="2" t="n">
-        <v>44630.246875</v>
-      </c>
-      <c r="BJ13" t="n">
-        <v>73.71099999999998</v>
-      </c>
-      <c r="BK13" t="n">
-        <v>0.0510881590977736</v>
-      </c>
-      <c r="BL13" t="n">
-        <v>15.026</v>
-      </c>
-      <c r="BM13" t="n">
-        <v>0.005163977794942631</v>
-      </c>
-      <c r="BN13" t="n">
-        <v>10.371</v>
-      </c>
-      <c r="BO13" t="n">
-        <v>0.01197218999737975</v>
-      </c>
-      <c r="BP13" s="2" t="n">
-        <v>44630.21150462963</v>
       </c>
     </row>
     <row r="14">
@@ -3254,7 +3213,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="2" t="n">
-        <v>44630.2434375</v>
+        <v>44630.25038194445</v>
       </c>
       <c r="D14" t="n">
         <v>981.197114609181</v>
@@ -3418,38 +3377,35 @@
       <c r="BE14" t="n">
         <v>10</v>
       </c>
-      <c r="BF14" s="2" t="n">
+      <c r="BF14" t="n">
+        <v>1026.5</v>
+      </c>
+      <c r="BG14" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH14" s="2" t="n">
+        <v>44630.25069444445</v>
+      </c>
+      <c r="BI14" t="n">
+        <v>73.71099999999998</v>
+      </c>
+      <c r="BJ14" t="n">
+        <v>0.0510881590977736</v>
+      </c>
+      <c r="BK14" t="n">
+        <v>15.026</v>
+      </c>
+      <c r="BL14" t="n">
+        <v>0.005163977794942631</v>
+      </c>
+      <c r="BM14" t="n">
+        <v>10.371</v>
+      </c>
+      <c r="BN14" t="n">
+        <v>0.01197218999737975</v>
+      </c>
+      <c r="BO14" s="2" t="n">
         <v>44630.25038194445</v>
-      </c>
-      <c r="BG14" t="n">
-        <v>1077.5</v>
-      </c>
-      <c r="BH14" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI14" s="2" t="n">
-        <v>44630.28229166667</v>
-      </c>
-      <c r="BJ14" t="n">
-        <v>94.03399999999999</v>
-      </c>
-      <c r="BK14" t="n">
-        <v>0.005163977794946705</v>
-      </c>
-      <c r="BL14" t="n">
-        <v>15.059</v>
-      </c>
-      <c r="BM14" t="n">
-        <v>0.003162277660168406</v>
-      </c>
-      <c r="BN14" t="n">
-        <v>14.104</v>
-      </c>
-      <c r="BO14" t="n">
-        <v>0.005163977794942655</v>
-      </c>
-      <c r="BP14" s="2" t="n">
-        <v>44630.24690972222</v>
       </c>
     </row>
     <row r="15">
@@ -3460,7 +3416,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>44630.27888888889</v>
+        <v>44630.28583333334</v>
       </c>
       <c r="D15" t="n">
         <v>1032.24950777739</v>
@@ -3624,38 +3580,35 @@
       <c r="BE15" t="n">
         <v>10</v>
       </c>
-      <c r="BF15" s="2" t="n">
+      <c r="BF15" t="n">
+        <v>1077.5</v>
+      </c>
+      <c r="BG15" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH15" s="2" t="n">
+        <v>44630.28611111111</v>
+      </c>
+      <c r="BI15" t="n">
+        <v>94.03399999999999</v>
+      </c>
+      <c r="BJ15" t="n">
+        <v>0.005163977794946705</v>
+      </c>
+      <c r="BK15" t="n">
+        <v>15.059</v>
+      </c>
+      <c r="BL15" t="n">
+        <v>0.003162277660168406</v>
+      </c>
+      <c r="BM15" t="n">
+        <v>14.104</v>
+      </c>
+      <c r="BN15" t="n">
+        <v>0.005163977794942655</v>
+      </c>
+      <c r="BO15" s="2" t="n">
         <v>44630.28583333334</v>
-      </c>
-      <c r="BG15" t="n">
-        <v>1128.5</v>
-      </c>
-      <c r="BH15" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI15" s="2" t="n">
-        <v>44630.31770833334</v>
-      </c>
-      <c r="BJ15" t="n">
-        <v>73.914</v>
-      </c>
-      <c r="BK15" t="n">
-        <v>0.056213877290219</v>
-      </c>
-      <c r="BL15" t="n">
-        <v>15</v>
-      </c>
-      <c r="BM15" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN15" t="n">
-        <v>10.389</v>
-      </c>
-      <c r="BO15" t="n">
-        <v>0.01100504934614667</v>
-      </c>
-      <c r="BP15" s="2" t="n">
-        <v>44630.28236111111</v>
       </c>
     </row>
     <row r="16">
@@ -3666,7 +3619,7 @@
         <v>15</v>
       </c>
       <c r="C16" s="2" t="n">
-        <v>44630.31440972222</v>
+        <v>44630.32135416667</v>
       </c>
       <c r="D16" t="n">
         <v>1083.40413598716</v>
@@ -3830,38 +3783,35 @@
       <c r="BE16" t="n">
         <v>10</v>
       </c>
-      <c r="BF16" s="2" t="n">
+      <c r="BF16" t="n">
+        <v>1128.5</v>
+      </c>
+      <c r="BG16" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH16" s="2" t="n">
+        <v>44630.32152777778</v>
+      </c>
+      <c r="BI16" t="n">
+        <v>73.914</v>
+      </c>
+      <c r="BJ16" t="n">
+        <v>0.056213877290219</v>
+      </c>
+      <c r="BK16" t="n">
+        <v>15</v>
+      </c>
+      <c r="BL16" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM16" t="n">
+        <v>10.389</v>
+      </c>
+      <c r="BN16" t="n">
+        <v>0.01100504934614667</v>
+      </c>
+      <c r="BO16" s="2" t="n">
         <v>44630.32135416667</v>
-      </c>
-      <c r="BG16" t="n">
-        <v>1180.5</v>
-      </c>
-      <c r="BH16" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI16" s="2" t="n">
-        <v>44630.35381944444</v>
-      </c>
-      <c r="BJ16" t="n">
-        <v>52.859</v>
-      </c>
-      <c r="BK16" t="n">
-        <v>0.01286683937708151</v>
-      </c>
-      <c r="BL16" t="n">
-        <v>15.001</v>
-      </c>
-      <c r="BM16" t="n">
-        <v>0.003162277660168406</v>
-      </c>
-      <c r="BN16" t="n">
-        <v>5.472</v>
-      </c>
-      <c r="BO16" t="n">
-        <v>0.004216370213558252</v>
-      </c>
-      <c r="BP16" s="2" t="n">
-        <v>44630.31788194444</v>
       </c>
     </row>
     <row r="17">
@@ -3872,7 +3822,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="2" t="n">
-        <v>44630.35003472222</v>
+        <v>44630.35697916667</v>
       </c>
       <c r="D17" t="n">
         <v>1134.69740568473</v>
@@ -4036,38 +3986,35 @@
       <c r="BE17" t="n">
         <v>10</v>
       </c>
-      <c r="BF17" s="2" t="n">
+      <c r="BF17" t="n">
+        <v>1180.5</v>
+      </c>
+      <c r="BG17" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH17" s="2" t="n">
+        <v>44630.35763888889</v>
+      </c>
+      <c r="BI17" t="n">
+        <v>52.859</v>
+      </c>
+      <c r="BJ17" t="n">
+        <v>0.01286683937708151</v>
+      </c>
+      <c r="BK17" t="n">
+        <v>15.001</v>
+      </c>
+      <c r="BL17" t="n">
+        <v>0.003162277660168406</v>
+      </c>
+      <c r="BM17" t="n">
+        <v>5.472</v>
+      </c>
+      <c r="BN17" t="n">
+        <v>0.004216370213558252</v>
+      </c>
+      <c r="BO17" s="2" t="n">
         <v>44630.35697916667</v>
-      </c>
-      <c r="BG17" t="n">
-        <v>1230.5</v>
-      </c>
-      <c r="BH17" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI17" s="2" t="n">
-        <v>44630.38854166667</v>
-      </c>
-      <c r="BJ17" t="n">
-        <v>31.96</v>
-      </c>
-      <c r="BK17" t="n">
-        <v>0.006666666666665278</v>
-      </c>
-      <c r="BL17" t="n">
-        <v>15.001</v>
-      </c>
-      <c r="BM17" t="n">
-        <v>0.003162277660168233</v>
-      </c>
-      <c r="BN17" t="n">
-        <v>-1.391</v>
-      </c>
-      <c r="BO17" t="n">
-        <v>0.003162277660168388</v>
-      </c>
-      <c r="BP17" s="2" t="n">
-        <v>44630.35350694445</v>
       </c>
     </row>
     <row r="18">
@@ -4078,7 +4025,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="2" t="n">
-        <v>44630.38537037037</v>
+        <v>44630.39231481482</v>
       </c>
       <c r="D18" t="n">
         <v>1185.58443154394</v>
@@ -4242,38 +4189,35 @@
       <c r="BE18" t="n">
         <v>10</v>
       </c>
-      <c r="BF18" s="2" t="n">
+      <c r="BF18" t="n">
+        <v>1230.5</v>
+      </c>
+      <c r="BG18" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH18" s="2" t="n">
+        <v>44630.39236111111</v>
+      </c>
+      <c r="BI18" t="n">
+        <v>31.96</v>
+      </c>
+      <c r="BJ18" t="n">
+        <v>0.006666666666665278</v>
+      </c>
+      <c r="BK18" t="n">
+        <v>15.001</v>
+      </c>
+      <c r="BL18" t="n">
+        <v>0.003162277660168233</v>
+      </c>
+      <c r="BM18" t="n">
+        <v>-1.391</v>
+      </c>
+      <c r="BN18" t="n">
+        <v>0.003162277660168388</v>
+      </c>
+      <c r="BO18" s="2" t="n">
         <v>44630.39231481482</v>
-      </c>
-      <c r="BG18" t="n">
-        <v>1281.5</v>
-      </c>
-      <c r="BH18" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI18" s="2" t="n">
-        <v>44630.42395833333</v>
-      </c>
-      <c r="BJ18" t="n">
-        <v>10.427</v>
-      </c>
-      <c r="BK18" t="n">
-        <v>0.004830458915396475</v>
-      </c>
-      <c r="BL18" t="n">
-        <v>15.01</v>
-      </c>
-      <c r="BM18" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN18" t="n">
-        <v>-14.207</v>
-      </c>
-      <c r="BO18" t="n">
-        <v>0.004830458915397131</v>
-      </c>
-      <c r="BP18" s="2" t="n">
-        <v>44630.38884259259</v>
       </c>
     </row>
     <row r="19">
@@ -4284,7 +4228,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="2" t="n">
-        <v>44630.42075231481</v>
+        <v>44630.42769675926</v>
       </c>
       <c r="D19" t="n">
         <v>1236.54344169795</v>
@@ -4448,38 +4392,35 @@
       <c r="BE19" t="n">
         <v>10</v>
       </c>
-      <c r="BF19" s="2" t="n">
+      <c r="BF19" t="n">
+        <v>1281.5</v>
+      </c>
+      <c r="BG19" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH19" s="2" t="n">
+        <v>44630.42777777778</v>
+      </c>
+      <c r="BI19" t="n">
+        <v>10.427</v>
+      </c>
+      <c r="BJ19" t="n">
+        <v>0.004830458915396475</v>
+      </c>
+      <c r="BK19" t="n">
+        <v>15.01</v>
+      </c>
+      <c r="BL19" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM19" t="n">
+        <v>-14.207</v>
+      </c>
+      <c r="BN19" t="n">
+        <v>0.004830458915397131</v>
+      </c>
+      <c r="BO19" s="2" t="n">
         <v>44630.42769675926</v>
-      </c>
-      <c r="BG19" t="n">
-        <v>1463.5</v>
-      </c>
-      <c r="BH19" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI19" s="2" t="n">
-        <v>44630.55034722222</v>
-      </c>
-      <c r="BJ19" t="n">
-        <v>10.294</v>
-      </c>
-      <c r="BK19" t="n">
-        <v>0.005163977794943815</v>
-      </c>
-      <c r="BL19" t="n">
-        <v>24.959</v>
-      </c>
-      <c r="BM19" t="n">
-        <v>0.003162277660168973</v>
-      </c>
-      <c r="BN19" t="n">
-        <v>-7.454000000000001</v>
-      </c>
-      <c r="BO19" t="n">
-        <v>0.005163977794942915</v>
-      </c>
-      <c r="BP19" s="2" t="n">
-        <v>44630.42422453704</v>
       </c>
     </row>
     <row r="20">
@@ -4490,7 +4431,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="2" t="n">
-        <v>44630.54678240741</v>
+        <v>44630.55372685185</v>
       </c>
       <c r="D20" t="n">
         <v>1418.01068783551</v>
@@ -4654,38 +4595,35 @@
       <c r="BE20" t="n">
         <v>10</v>
       </c>
-      <c r="BF20" s="2" t="n">
+      <c r="BF20" t="n">
+        <v>1463.5</v>
+      </c>
+      <c r="BG20" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH20" s="2" t="n">
+        <v>44630.55416666667</v>
+      </c>
+      <c r="BI20" t="n">
+        <v>10.294</v>
+      </c>
+      <c r="BJ20" t="n">
+        <v>0.005163977794943815</v>
+      </c>
+      <c r="BK20" t="n">
+        <v>24.959</v>
+      </c>
+      <c r="BL20" t="n">
+        <v>0.003162277660168973</v>
+      </c>
+      <c r="BM20" t="n">
+        <v>-7.454000000000001</v>
+      </c>
+      <c r="BN20" t="n">
+        <v>0.005163977794942915</v>
+      </c>
+      <c r="BO20" s="2" t="n">
         <v>44630.55372685185</v>
-      </c>
-      <c r="BG20" t="n">
-        <v>1553.5</v>
-      </c>
-      <c r="BH20" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI20" s="2" t="n">
-        <v>44630.61284722222</v>
-      </c>
-      <c r="BJ20" t="n">
-        <v>31.646</v>
-      </c>
-      <c r="BK20" t="n">
-        <v>0.04742245131674375</v>
-      </c>
-      <c r="BL20" t="n">
-        <v>24.96</v>
-      </c>
-      <c r="BM20" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN20" t="n">
-        <v>6.972999999999999</v>
-      </c>
-      <c r="BO20" t="n">
-        <v>0.02162817093001107</v>
-      </c>
-      <c r="BP20" s="2" t="n">
-        <v>44630.55025462963</v>
       </c>
     </row>
     <row r="21">
@@ -4696,7 +4634,7 @@
         <v>20</v>
       </c>
       <c r="C21" s="2" t="n">
-        <v>44630.60905092592</v>
+        <v>44630.61599537037</v>
       </c>
       <c r="D21" t="n">
         <v>1507.68438923358</v>
@@ -4860,38 +4798,35 @@
       <c r="BE21" t="n">
         <v>10</v>
       </c>
-      <c r="BF21" s="2" t="n">
+      <c r="BF21" t="n">
+        <v>1553.5</v>
+      </c>
+      <c r="BG21" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH21" s="2" t="n">
+        <v>44630.61666666667</v>
+      </c>
+      <c r="BI21" t="n">
+        <v>31.646</v>
+      </c>
+      <c r="BJ21" t="n">
+        <v>0.04742245131674375</v>
+      </c>
+      <c r="BK21" t="n">
+        <v>24.96</v>
+      </c>
+      <c r="BL21" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM21" t="n">
+        <v>6.972999999999999</v>
+      </c>
+      <c r="BN21" t="n">
+        <v>0.02162817093001107</v>
+      </c>
+      <c r="BO21" s="2" t="n">
         <v>44630.61599537037</v>
-      </c>
-      <c r="BG21" t="n">
-        <v>1603.5</v>
-      </c>
-      <c r="BH21" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI21" s="2" t="n">
-        <v>44630.64756944445</v>
-      </c>
-      <c r="BJ21" t="n">
-        <v>52.38200000000001</v>
-      </c>
-      <c r="BK21" t="n">
-        <v>0.007888106377467436</v>
-      </c>
-      <c r="BL21" t="n">
-        <v>24.97</v>
-      </c>
-      <c r="BM21" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN21" t="n">
-        <v>14.551</v>
-      </c>
-      <c r="BO21" t="n">
-        <v>0.003162277660167556</v>
-      </c>
-      <c r="BP21" s="2" t="n">
-        <v>44630.61252314815</v>
       </c>
     </row>
     <row r="22">
@@ -4902,7 +4837,7 @@
         <v>21</v>
       </c>
       <c r="C22" s="2" t="n">
-        <v>44630.64409722222</v>
+        <v>44630.65104166666</v>
       </c>
       <c r="D22" t="n">
         <v>1558.15084213018</v>
@@ -5066,38 +5001,35 @@
       <c r="BE22" t="n">
         <v>10</v>
       </c>
-      <c r="BF22" s="2" t="n">
+      <c r="BF22" t="n">
+        <v>1603.5</v>
+      </c>
+      <c r="BG22" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH22" s="2" t="n">
+        <v>44630.65138888889</v>
+      </c>
+      <c r="BI22" t="n">
+        <v>52.38200000000001</v>
+      </c>
+      <c r="BJ22" t="n">
+        <v>0.007888106377467436</v>
+      </c>
+      <c r="BK22" t="n">
+        <v>24.97</v>
+      </c>
+      <c r="BL22" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM22" t="n">
+        <v>14.551</v>
+      </c>
+      <c r="BN22" t="n">
+        <v>0.003162277660167556</v>
+      </c>
+      <c r="BO22" s="2" t="n">
         <v>44630.65104166666</v>
-      </c>
-      <c r="BG22" t="n">
-        <v>1654.5</v>
-      </c>
-      <c r="BH22" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI22" s="2" t="n">
-        <v>44630.68298611111</v>
-      </c>
-      <c r="BJ22" t="n">
-        <v>73.39099999999999</v>
-      </c>
-      <c r="BK22" t="n">
-        <v>0.009944289260122441</v>
-      </c>
-      <c r="BL22" t="n">
-        <v>24.98</v>
-      </c>
-      <c r="BM22" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN22" t="n">
-        <v>19.894</v>
-      </c>
-      <c r="BO22" t="n">
-        <v>0.005163977794942218</v>
-      </c>
-      <c r="BP22" s="2" t="n">
-        <v>44630.64756944445</v>
       </c>
     </row>
     <row r="23">
@@ -5108,7 +5040,7 @@
         <v>22</v>
       </c>
       <c r="C23" s="2" t="n">
-        <v>44630.67949074074</v>
+        <v>44630.68643518518</v>
       </c>
       <c r="D23" t="n">
         <v>1609.11343614757</v>
@@ -5272,38 +5204,35 @@
       <c r="BE23" t="n">
         <v>10</v>
       </c>
-      <c r="BF23" s="2" t="n">
+      <c r="BF23" t="n">
+        <v>1654.5</v>
+      </c>
+      <c r="BG23" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH23" s="2" t="n">
+        <v>44630.68680555555</v>
+      </c>
+      <c r="BI23" t="n">
+        <v>73.39099999999999</v>
+      </c>
+      <c r="BJ23" t="n">
+        <v>0.009944289260122441</v>
+      </c>
+      <c r="BK23" t="n">
+        <v>24.98</v>
+      </c>
+      <c r="BL23" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM23" t="n">
+        <v>19.894</v>
+      </c>
+      <c r="BN23" t="n">
+        <v>0.005163977794942218</v>
+      </c>
+      <c r="BO23" s="2" t="n">
         <v>44630.68643518518</v>
-      </c>
-      <c r="BG23" t="n">
-        <v>1705.5</v>
-      </c>
-      <c r="BH23" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI23" s="2" t="n">
-        <v>44630.71840277778</v>
-      </c>
-      <c r="BJ23" t="n">
-        <v>93.56800000000001</v>
-      </c>
-      <c r="BK23" t="n">
-        <v>0.01032795558988404</v>
-      </c>
-      <c r="BL23" t="n">
-        <v>25.02</v>
-      </c>
-      <c r="BM23" t="n">
-        <v>0.004714045207911161</v>
-      </c>
-      <c r="BN23" t="n">
-        <v>23.912</v>
-      </c>
-      <c r="BO23" t="n">
-        <v>0.004216370213558046</v>
-      </c>
-      <c r="BP23" s="2" t="n">
-        <v>44630.68296296296</v>
       </c>
     </row>
     <row r="24">
@@ -5314,7 +5243,7 @@
         <v>23</v>
       </c>
       <c r="C24" s="2" t="n">
-        <v>44630.71466435185</v>
+        <v>44630.7216087963</v>
       </c>
       <c r="D24" t="n">
         <v>1659.77526769787</v>
@@ -5478,38 +5407,35 @@
       <c r="BE24" t="n">
         <v>10</v>
       </c>
-      <c r="BF24" s="2" t="n">
+      <c r="BF24" t="n">
+        <v>1705.5</v>
+      </c>
+      <c r="BG24" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH24" s="2" t="n">
+        <v>44630.72222222222</v>
+      </c>
+      <c r="BI24" t="n">
+        <v>93.56800000000001</v>
+      </c>
+      <c r="BJ24" t="n">
+        <v>0.01032795558988404</v>
+      </c>
+      <c r="BK24" t="n">
+        <v>25.02</v>
+      </c>
+      <c r="BL24" t="n">
+        <v>0.004714045207911161</v>
+      </c>
+      <c r="BM24" t="n">
+        <v>23.912</v>
+      </c>
+      <c r="BN24" t="n">
+        <v>0.004216370213558046</v>
+      </c>
+      <c r="BO24" s="2" t="n">
         <v>44630.7216087963</v>
-      </c>
-      <c r="BG24" t="n">
-        <v>1755.5</v>
-      </c>
-      <c r="BH24" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI24" s="2" t="n">
-        <v>44630.753125</v>
-      </c>
-      <c r="BJ24" t="n">
-        <v>73.58700000000002</v>
-      </c>
-      <c r="BK24" t="n">
-        <v>0.0156702123647253</v>
-      </c>
-      <c r="BL24" t="n">
-        <v>24.948</v>
-      </c>
-      <c r="BM24" t="n">
-        <v>0.004216370213556054</v>
-      </c>
-      <c r="BN24" t="n">
-        <v>19.901</v>
-      </c>
-      <c r="BO24" t="n">
-        <v>0.003162277660169602</v>
-      </c>
-      <c r="BP24" s="2" t="n">
-        <v>44630.71813657408</v>
       </c>
     </row>
     <row r="25">
@@ -5520,7 +5446,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="2" t="n">
-        <v>44630.74993055555</v>
+        <v>44630.756875</v>
       </c>
       <c r="D25" t="n">
         <v>1710.55661348998</v>
@@ -5684,38 +5610,35 @@
       <c r="BE25" t="n">
         <v>10</v>
       </c>
-      <c r="BF25" s="2" t="n">
+      <c r="BF25" t="n">
+        <v>1755.5</v>
+      </c>
+      <c r="BG25" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH25" s="2" t="n">
+        <v>44630.75694444445</v>
+      </c>
+      <c r="BI25" t="n">
+        <v>73.58700000000002</v>
+      </c>
+      <c r="BJ25" t="n">
+        <v>0.0156702123647253</v>
+      </c>
+      <c r="BK25" t="n">
+        <v>24.948</v>
+      </c>
+      <c r="BL25" t="n">
+        <v>0.004216370213556054</v>
+      </c>
+      <c r="BM25" t="n">
+        <v>19.901</v>
+      </c>
+      <c r="BN25" t="n">
+        <v>0.003162277660169602</v>
+      </c>
+      <c r="BO25" s="2" t="n">
         <v>44630.756875</v>
-      </c>
-      <c r="BG25" t="n">
-        <v>1806.5</v>
-      </c>
-      <c r="BH25" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI25" s="2" t="n">
-        <v>44630.78854166667</v>
-      </c>
-      <c r="BJ25" t="n">
-        <v>52.601</v>
-      </c>
-      <c r="BK25" t="n">
-        <v>0.0375499667110433</v>
-      </c>
-      <c r="BL25" t="n">
-        <v>24.95</v>
-      </c>
-      <c r="BM25" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN25" t="n">
-        <v>14.596</v>
-      </c>
-      <c r="BO25" t="n">
-        <v>0.01173787790777326</v>
-      </c>
-      <c r="BP25" s="2" t="n">
-        <v>44630.75340277778</v>
       </c>
     </row>
     <row r="26">
@@ -5726,7 +5649,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="2" t="n">
-        <v>44630.78523148148</v>
+        <v>44630.79217592593</v>
       </c>
       <c r="D26" t="n">
         <v>1761.37755522504</v>
@@ -5890,38 +5813,35 @@
       <c r="BE26" t="n">
         <v>10</v>
       </c>
-      <c r="BF26" s="2" t="n">
+      <c r="BF26" t="n">
+        <v>1806.5</v>
+      </c>
+      <c r="BG26" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH26" s="2" t="n">
+        <v>44630.79236111111</v>
+      </c>
+      <c r="BI26" t="n">
+        <v>52.601</v>
+      </c>
+      <c r="BJ26" t="n">
+        <v>0.0375499667110433</v>
+      </c>
+      <c r="BK26" t="n">
+        <v>24.95</v>
+      </c>
+      <c r="BL26" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM26" t="n">
+        <v>14.596</v>
+      </c>
+      <c r="BN26" t="n">
+        <v>0.01173787790777326</v>
+      </c>
+      <c r="BO26" s="2" t="n">
         <v>44630.79217592593</v>
-      </c>
-      <c r="BG26" t="n">
-        <v>1857.5</v>
-      </c>
-      <c r="BH26" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI26" s="2" t="n">
-        <v>44630.82395833333</v>
-      </c>
-      <c r="BJ26" t="n">
-        <v>31.79500000000001</v>
-      </c>
-      <c r="BK26" t="n">
-        <v>0.005270462766946917</v>
-      </c>
-      <c r="BL26" t="n">
-        <v>24.95</v>
-      </c>
-      <c r="BM26" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN26" t="n">
-        <v>7.029999999999999</v>
-      </c>
-      <c r="BO26" t="n">
-        <v>0</v>
-      </c>
-      <c r="BP26" s="2" t="n">
-        <v>44630.78870370371</v>
       </c>
     </row>
     <row r="27">
@@ -5932,7 +5852,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="2" t="n">
-        <v>44630.82030092592</v>
+        <v>44630.82724537037</v>
       </c>
       <c r="D27" t="n">
         <v>1811.88126775622</v>
@@ -6096,38 +6016,35 @@
       <c r="BE27" t="n">
         <v>10</v>
       </c>
-      <c r="BF27" s="2" t="n">
+      <c r="BF27" t="n">
+        <v>1857.5</v>
+      </c>
+      <c r="BG27" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH27" s="2" t="n">
+        <v>44630.82777777778</v>
+      </c>
+      <c r="BI27" t="n">
+        <v>31.79500000000001</v>
+      </c>
+      <c r="BJ27" t="n">
+        <v>0.005270462766946917</v>
+      </c>
+      <c r="BK27" t="n">
+        <v>24.95</v>
+      </c>
+      <c r="BL27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM27" t="n">
+        <v>7.029999999999999</v>
+      </c>
+      <c r="BN27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO27" s="2" t="n">
         <v>44630.82724537037</v>
-      </c>
-      <c r="BG27" t="n">
-        <v>1907.5</v>
-      </c>
-      <c r="BH27" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI27" s="2" t="n">
-        <v>44630.85868055555</v>
-      </c>
-      <c r="BJ27" t="n">
-        <v>10.317</v>
-      </c>
-      <c r="BK27" t="n">
-        <v>0.006749485577105444</v>
-      </c>
-      <c r="BL27" t="n">
-        <v>24.953</v>
-      </c>
-      <c r="BM27" t="n">
-        <v>0.004830458915396404</v>
-      </c>
-      <c r="BN27" t="n">
-        <v>-7.429999999999998</v>
-      </c>
-      <c r="BO27" t="n">
-        <v>0.00816496580927724</v>
-      </c>
-      <c r="BP27" s="2" t="n">
-        <v>44630.82377314815</v>
       </c>
     </row>
     <row r="28">
@@ -6138,7 +6055,7 @@
         <v>27</v>
       </c>
       <c r="C28" s="2" t="n">
-        <v>44630.8554050926</v>
+        <v>44630.86234953703</v>
       </c>
       <c r="D28" t="n">
         <v>1862.43707663565</v>
@@ -6302,38 +6219,35 @@
       <c r="BE28" t="n">
         <v>10</v>
       </c>
-      <c r="BF28" s="2" t="n">
+      <c r="BF28" t="n">
+        <v>1907.5</v>
+      </c>
+      <c r="BG28" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH28" s="2" t="n">
+        <v>44630.8625</v>
+      </c>
+      <c r="BI28" t="n">
+        <v>10.317</v>
+      </c>
+      <c r="BJ28" t="n">
+        <v>0.006749485577105444</v>
+      </c>
+      <c r="BK28" t="n">
+        <v>24.953</v>
+      </c>
+      <c r="BL28" t="n">
+        <v>0.004830458915396404</v>
+      </c>
+      <c r="BM28" t="n">
+        <v>-7.429999999999998</v>
+      </c>
+      <c r="BN28" t="n">
+        <v>0.00816496580927724</v>
+      </c>
+      <c r="BO28" s="2" t="n">
         <v>44630.86234953703</v>
-      </c>
-      <c r="BG28" t="n">
-        <v>2088.5</v>
-      </c>
-      <c r="BH28" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI28" s="2" t="n">
-        <v>44630.984375</v>
-      </c>
-      <c r="BJ28" t="n">
-        <v>10.232</v>
-      </c>
-      <c r="BK28" t="n">
-        <v>0.01135292424395046</v>
-      </c>
-      <c r="BL28" t="n">
-        <v>34.95</v>
-      </c>
-      <c r="BM28" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN28" t="n">
-        <v>-0.769</v>
-      </c>
-      <c r="BO28" t="n">
-        <v>0.01197218999737867</v>
-      </c>
-      <c r="BP28" s="2" t="n">
-        <v>44630.85887731481</v>
       </c>
     </row>
     <row r="29">
@@ -6344,7 +6258,7 @@
         <v>28</v>
       </c>
       <c r="C29" s="2" t="n">
-        <v>44630.9809375</v>
+        <v>44630.98788194444</v>
       </c>
       <c r="D29" t="n">
         <v>2043.19406015425</v>
@@ -6508,38 +6422,35 @@
       <c r="BE29" t="n">
         <v>10</v>
       </c>
-      <c r="BF29" s="2" t="n">
+      <c r="BF29" t="n">
+        <v>2088.5</v>
+      </c>
+      <c r="BG29" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH29" s="2" t="n">
+        <v>44630.98819444444</v>
+      </c>
+      <c r="BI29" t="n">
+        <v>10.232</v>
+      </c>
+      <c r="BJ29" t="n">
+        <v>0.01135292424395046</v>
+      </c>
+      <c r="BK29" t="n">
+        <v>34.95</v>
+      </c>
+      <c r="BL29" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM29" t="n">
+        <v>-0.769</v>
+      </c>
+      <c r="BN29" t="n">
+        <v>0.01197218999737867</v>
+      </c>
+      <c r="BO29" s="2" t="n">
         <v>44630.98788194444</v>
-      </c>
-      <c r="BG29" t="n">
-        <v>2139.5</v>
-      </c>
-      <c r="BH29" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI29" s="2" t="n">
-        <v>44631.01979166667</v>
-      </c>
-      <c r="BJ29" t="n">
-        <v>31.628</v>
-      </c>
-      <c r="BK29" t="n">
-        <v>0.06646636576328076</v>
-      </c>
-      <c r="BL29" t="n">
-        <v>34.95999999999999</v>
-      </c>
-      <c r="BM29" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN29" t="n">
-        <v>15.624</v>
-      </c>
-      <c r="BO29" t="n">
-        <v>0.03169297153067958</v>
-      </c>
-      <c r="BP29" s="2" t="n">
-        <v>44630.98440972222</v>
       </c>
     </row>
     <row r="30">
@@ -6550,7 +6461,7 @@
         <v>29</v>
       </c>
       <c r="C30" s="2" t="n">
-        <v>44631.01645833333</v>
+        <v>44631.02340277778</v>
       </c>
       <c r="D30" t="n">
         <v>2094.35164161771</v>
@@ -6714,38 +6625,35 @@
       <c r="BE30" t="n">
         <v>10</v>
       </c>
-      <c r="BF30" s="2" t="n">
+      <c r="BF30" t="n">
+        <v>2139.5</v>
+      </c>
+      <c r="BG30" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH30" s="2" t="n">
+        <v>44631.02361111111</v>
+      </c>
+      <c r="BI30" t="n">
+        <v>31.628</v>
+      </c>
+      <c r="BJ30" t="n">
+        <v>0.06646636576328076</v>
+      </c>
+      <c r="BK30" t="n">
+        <v>34.95999999999999</v>
+      </c>
+      <c r="BL30" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM30" t="n">
+        <v>15.624</v>
+      </c>
+      <c r="BN30" t="n">
+        <v>0.03169297153067958</v>
+      </c>
+      <c r="BO30" s="2" t="n">
         <v>44631.02340277778</v>
-      </c>
-      <c r="BG30" t="n">
-        <v>2191.5</v>
-      </c>
-      <c r="BH30" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI30" s="2" t="n">
-        <v>44631.05590277778</v>
-      </c>
-      <c r="BJ30" t="n">
-        <v>52.389</v>
-      </c>
-      <c r="BK30" t="n">
-        <v>0.01911950719959794</v>
-      </c>
-      <c r="BL30" t="n">
-        <v>34.971</v>
-      </c>
-      <c r="BM30" t="n">
-        <v>0.003162277660167307</v>
-      </c>
-      <c r="BN30" t="n">
-        <v>23.768</v>
-      </c>
-      <c r="BO30" t="n">
-        <v>0.006324555320336114</v>
-      </c>
-      <c r="BP30" s="2" t="n">
-        <v>44631.01993055556</v>
       </c>
     </row>
     <row r="31">
@@ -6756,7 +6664,7 @@
         <v>30</v>
       </c>
       <c r="C31" s="2" t="n">
-        <v>44631.05226851852</v>
+        <v>44631.05921296297</v>
       </c>
       <c r="D31" t="n">
         <v>2145.92001368105</v>
@@ -6920,38 +6828,35 @@
       <c r="BE31" t="n">
         <v>10</v>
       </c>
-      <c r="BF31" s="2" t="n">
+      <c r="BF31" t="n">
+        <v>2191.5</v>
+      </c>
+      <c r="BG31" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH31" s="2" t="n">
+        <v>44631.05972222222</v>
+      </c>
+      <c r="BI31" t="n">
+        <v>52.389</v>
+      </c>
+      <c r="BJ31" t="n">
+        <v>0.01911950719959794</v>
+      </c>
+      <c r="BK31" t="n">
+        <v>34.971</v>
+      </c>
+      <c r="BL31" t="n">
+        <v>0.003162277660167307</v>
+      </c>
+      <c r="BM31" t="n">
+        <v>23.768</v>
+      </c>
+      <c r="BN31" t="n">
+        <v>0.006324555320336114</v>
+      </c>
+      <c r="BO31" s="2" t="n">
         <v>44631.05921296297</v>
-      </c>
-      <c r="BG31" t="n">
-        <v>2241.5</v>
-      </c>
-      <c r="BH31" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI31" s="2" t="n">
-        <v>44631.090625</v>
-      </c>
-      <c r="BJ31" t="n">
-        <v>73.33500000000001</v>
-      </c>
-      <c r="BK31" t="n">
-        <v>0.01080123449734803</v>
-      </c>
-      <c r="BL31" t="n">
-        <v>34.99</v>
-      </c>
-      <c r="BM31" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN31" t="n">
-        <v>29.5</v>
-      </c>
-      <c r="BO31" t="n">
-        <v>0</v>
-      </c>
-      <c r="BP31" s="2" t="n">
-        <v>44631.05574074074</v>
       </c>
     </row>
     <row r="32">
@@ -6962,7 +6867,7 @@
         <v>31</v>
       </c>
       <c r="C32" s="2" t="n">
-        <v>44631.08709490741</v>
+        <v>44631.09403935185</v>
       </c>
       <c r="D32" t="n">
         <v>2196.07408450916</v>
@@ -7126,38 +7031,35 @@
       <c r="BE32" t="n">
         <v>10</v>
       </c>
-      <c r="BF32" s="2" t="n">
+      <c r="BF32" t="n">
+        <v>2241.5</v>
+      </c>
+      <c r="BG32" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH32" s="2" t="n">
+        <v>44631.09444444445</v>
+      </c>
+      <c r="BI32" t="n">
+        <v>73.33500000000001</v>
+      </c>
+      <c r="BJ32" t="n">
+        <v>0.01080123449734803</v>
+      </c>
+      <c r="BK32" t="n">
+        <v>34.99</v>
+      </c>
+      <c r="BL32" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM32" t="n">
+        <v>29.5</v>
+      </c>
+      <c r="BN32" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO32" s="2" t="n">
         <v>44631.09403935185</v>
-      </c>
-      <c r="BG32" t="n">
-        <v>2291.5</v>
-      </c>
-      <c r="BH32" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI32" s="2" t="n">
-        <v>44631.12534722222</v>
-      </c>
-      <c r="BJ32" t="n">
-        <v>93.25399999999999</v>
-      </c>
-      <c r="BK32" t="n">
-        <v>0.016465452046975</v>
-      </c>
-      <c r="BL32" t="n">
-        <v>35.041</v>
-      </c>
-      <c r="BM32" t="n">
-        <v>0.005676462121977799</v>
-      </c>
-      <c r="BN32" t="n">
-        <v>33.79600000000001</v>
-      </c>
-      <c r="BO32" t="n">
-        <v>0.005163977794942743</v>
-      </c>
-      <c r="BP32" s="2" t="n">
-        <v>44631.09056712963</v>
       </c>
     </row>
     <row r="33">
@@ -7168,7 +7070,7 @@
         <v>32</v>
       </c>
       <c r="C33" s="2" t="n">
-        <v>44631.12181712963</v>
+        <v>44631.12876157407</v>
       </c>
       <c r="D33" t="n">
         <v>2246.06822838634</v>
@@ -7332,38 +7234,35 @@
       <c r="BE33" t="n">
         <v>10</v>
       </c>
-      <c r="BF33" s="2" t="n">
+      <c r="BF33" t="n">
+        <v>2291.5</v>
+      </c>
+      <c r="BG33" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH33" s="2" t="n">
+        <v>44631.12916666667</v>
+      </c>
+      <c r="BI33" t="n">
+        <v>93.25399999999999</v>
+      </c>
+      <c r="BJ33" t="n">
+        <v>0.016465452046975</v>
+      </c>
+      <c r="BK33" t="n">
+        <v>35.041</v>
+      </c>
+      <c r="BL33" t="n">
+        <v>0.005676462121977799</v>
+      </c>
+      <c r="BM33" t="n">
+        <v>33.79600000000001</v>
+      </c>
+      <c r="BN33" t="n">
+        <v>0.005163977794942743</v>
+      </c>
+      <c r="BO33" s="2" t="n">
         <v>44631.12876157407</v>
-      </c>
-      <c r="BG33" t="n">
-        <v>2341.5</v>
-      </c>
-      <c r="BH33" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI33" s="2" t="n">
-        <v>44631.16006944444</v>
-      </c>
-      <c r="BJ33" t="n">
-        <v>73.53999999999999</v>
-      </c>
-      <c r="BK33" t="n">
-        <v>0.02624669291337254</v>
-      </c>
-      <c r="BL33" t="n">
-        <v>34.94499999999999</v>
-      </c>
-      <c r="BM33" t="n">
-        <v>0.005270462766950217</v>
-      </c>
-      <c r="BN33" t="n">
-        <v>29.507</v>
-      </c>
-      <c r="BO33" t="n">
-        <v>0.008232726023486557</v>
-      </c>
-      <c r="BP33" s="2" t="n">
-        <v>44631.12528935185</v>
       </c>
     </row>
     <row r="34">
@@ -7374,7 +7273,7 @@
         <v>33</v>
       </c>
       <c r="C34" s="2" t="n">
-        <v>44631.15667824074</v>
+        <v>44631.16362268518</v>
       </c>
       <c r="D34" t="n">
         <v>2296.26566246151</v>
@@ -7538,38 +7437,35 @@
       <c r="BE34" t="n">
         <v>10</v>
       </c>
-      <c r="BF34" s="2" t="n">
+      <c r="BF34" t="n">
+        <v>2341.5</v>
+      </c>
+      <c r="BG34" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH34" s="2" t="n">
+        <v>44631.16388888889</v>
+      </c>
+      <c r="BI34" t="n">
+        <v>73.53999999999999</v>
+      </c>
+      <c r="BJ34" t="n">
+        <v>0.02624669291337254</v>
+      </c>
+      <c r="BK34" t="n">
+        <v>34.94499999999999</v>
+      </c>
+      <c r="BL34" t="n">
+        <v>0.005270462766950217</v>
+      </c>
+      <c r="BM34" t="n">
+        <v>29.507</v>
+      </c>
+      <c r="BN34" t="n">
+        <v>0.008232726023486557</v>
+      </c>
+      <c r="BO34" s="2" t="n">
         <v>44631.16362268518</v>
-      </c>
-      <c r="BG34" t="n">
-        <v>2392.5</v>
-      </c>
-      <c r="BH34" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI34" s="2" t="n">
-        <v>44631.19548611111</v>
-      </c>
-      <c r="BJ34" t="n">
-        <v>52.496</v>
-      </c>
-      <c r="BK34" t="n">
-        <v>0.01074967699773214</v>
-      </c>
-      <c r="BL34" t="n">
-        <v>34.941</v>
-      </c>
-      <c r="BM34" t="n">
-        <v>0.0031622776601692</v>
-      </c>
-      <c r="BN34" t="n">
-        <v>23.777</v>
-      </c>
-      <c r="BO34" t="n">
-        <v>0.004830458915398123</v>
-      </c>
-      <c r="BP34" s="2" t="n">
-        <v>44631.16015046297</v>
       </c>
     </row>
     <row r="35">
@@ -7580,7 +7476,7 @@
         <v>34</v>
       </c>
       <c r="C35" s="2" t="n">
-        <v>44631.19170138889</v>
+        <v>44631.19864583333</v>
       </c>
       <c r="D35" t="n">
         <v>2346.70108120143</v>
@@ -7744,38 +7640,35 @@
       <c r="BE35" t="n">
         <v>10</v>
       </c>
-      <c r="BF35" s="2" t="n">
+      <c r="BF35" t="n">
+        <v>2392.5</v>
+      </c>
+      <c r="BG35" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH35" s="2" t="n">
+        <v>44631.19930555556</v>
+      </c>
+      <c r="BI35" t="n">
+        <v>52.496</v>
+      </c>
+      <c r="BJ35" t="n">
+        <v>0.01074967699773214</v>
+      </c>
+      <c r="BK35" t="n">
+        <v>34.941</v>
+      </c>
+      <c r="BL35" t="n">
+        <v>0.0031622776601692</v>
+      </c>
+      <c r="BM35" t="n">
+        <v>23.777</v>
+      </c>
+      <c r="BN35" t="n">
+        <v>0.004830458915398123</v>
+      </c>
+      <c r="BO35" s="2" t="n">
         <v>44631.19864583333</v>
-      </c>
-      <c r="BG35" t="n">
-        <v>2443.5</v>
-      </c>
-      <c r="BH35" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI35" s="2" t="n">
-        <v>44631.23090277778</v>
-      </c>
-      <c r="BJ35" t="n">
-        <v>31.712</v>
-      </c>
-      <c r="BK35" t="n">
-        <v>0.02616188916046516</v>
-      </c>
-      <c r="BL35" t="n">
-        <v>34.94</v>
-      </c>
-      <c r="BM35" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN35" t="n">
-        <v>15.645</v>
-      </c>
-      <c r="BO35" t="n">
-        <v>0.01354006400772616</v>
-      </c>
-      <c r="BP35" s="2" t="n">
-        <v>44631.19517361111</v>
       </c>
     </row>
     <row r="36">
@@ -7786,7 +7679,7 @@
         <v>35</v>
       </c>
       <c r="C36" s="2" t="n">
-        <v>44631.22761574074</v>
+        <v>44631.23456018518</v>
       </c>
       <c r="D36" t="n">
         <v>2398.41770924627</v>
@@ -7950,38 +7843,35 @@
       <c r="BE36" t="n">
         <v>10</v>
       </c>
-      <c r="BF36" s="2" t="n">
+      <c r="BF36" t="n">
+        <v>2443.5</v>
+      </c>
+      <c r="BG36" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH36" s="2" t="n">
+        <v>44631.23472222222</v>
+      </c>
+      <c r="BI36" t="n">
+        <v>31.712</v>
+      </c>
+      <c r="BJ36" t="n">
+        <v>0.02616188916046516</v>
+      </c>
+      <c r="BK36" t="n">
+        <v>34.94</v>
+      </c>
+      <c r="BL36" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM36" t="n">
+        <v>15.645</v>
+      </c>
+      <c r="BN36" t="n">
+        <v>0.01354006400772616</v>
+      </c>
+      <c r="BO36" s="2" t="n">
         <v>44631.23456018518</v>
-      </c>
-      <c r="BG36" t="n">
-        <v>2493.5</v>
-      </c>
-      <c r="BH36" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI36" s="2" t="n">
-        <v>44631.265625</v>
-      </c>
-      <c r="BJ36" t="n">
-        <v>10.269</v>
-      </c>
-      <c r="BK36" t="n">
-        <v>0.007378647873725878</v>
-      </c>
-      <c r="BL36" t="n">
-        <v>34.94</v>
-      </c>
-      <c r="BM36" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN36" t="n">
-        <v>-0.7370000000000001</v>
-      </c>
-      <c r="BO36" t="n">
-        <v>0.009486832980505148</v>
-      </c>
-      <c r="BP36" s="2" t="n">
-        <v>44631.23108796297</v>
       </c>
     </row>
     <row r="37">
@@ -7992,7 +7882,7 @@
         <v>36</v>
       </c>
       <c r="C37" s="2" t="n">
-        <v>44631.26237268518</v>
+        <v>44631.26931712963</v>
       </c>
       <c r="D37" t="n">
         <v>2448.4667468518</v>
@@ -8156,38 +8046,35 @@
       <c r="BE37" t="n">
         <v>10</v>
       </c>
-      <c r="BF37" s="2" t="n">
+      <c r="BF37" t="n">
+        <v>2493.5</v>
+      </c>
+      <c r="BG37" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH37" s="2" t="n">
+        <v>44631.26944444444</v>
+      </c>
+      <c r="BI37" t="n">
+        <v>10.269</v>
+      </c>
+      <c r="BJ37" t="n">
+        <v>0.007378647873725878</v>
+      </c>
+      <c r="BK37" t="n">
+        <v>34.94</v>
+      </c>
+      <c r="BL37" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM37" t="n">
+        <v>-0.7370000000000001</v>
+      </c>
+      <c r="BN37" t="n">
+        <v>0.009486832980505148</v>
+      </c>
+      <c r="BO37" s="2" t="n">
         <v>44631.26931712963</v>
-      </c>
-      <c r="BG37" t="n">
-        <v>2794.5</v>
-      </c>
-      <c r="BH37" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI37" s="2" t="n">
-        <v>44631.47465277778</v>
-      </c>
-      <c r="BJ37" t="n">
-        <v>10.145</v>
-      </c>
-      <c r="BK37" t="n">
-        <v>0.005270462766947264</v>
-      </c>
-      <c r="BL37" t="n">
-        <v>44.93</v>
-      </c>
-      <c r="BM37" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN37" t="n">
-        <v>6.51</v>
-      </c>
-      <c r="BO37" t="n">
-        <v>0.006666666666666251</v>
-      </c>
-      <c r="BP37" s="2" t="n">
-        <v>44631.26584490741</v>
       </c>
     </row>
     <row r="38">
@@ -8198,7 +8085,7 @@
         <v>37</v>
       </c>
       <c r="C38" s="2" t="n">
-        <v>44631.47142361111</v>
+        <v>44631.47836805556</v>
       </c>
       <c r="D38" t="n">
         <v>2749.4988008663</v>
@@ -8362,38 +8249,35 @@
       <c r="BE38" t="n">
         <v>10</v>
       </c>
-      <c r="BF38" s="2" t="n">
+      <c r="BF38" t="n">
+        <v>2794.5</v>
+      </c>
+      <c r="BG38" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH38" s="2" t="n">
+        <v>44631.47847222222</v>
+      </c>
+      <c r="BI38" t="n">
+        <v>10.145</v>
+      </c>
+      <c r="BJ38" t="n">
+        <v>0.005270462766947264</v>
+      </c>
+      <c r="BK38" t="n">
+        <v>44.93</v>
+      </c>
+      <c r="BL38" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM38" t="n">
+        <v>6.51</v>
+      </c>
+      <c r="BN38" t="n">
+        <v>0.006666666666666251</v>
+      </c>
+      <c r="BO38" s="2" t="n">
         <v>44631.47836805556</v>
-      </c>
-      <c r="BG38" t="n">
-        <v>2845.5</v>
-      </c>
-      <c r="BH38" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI38" s="2" t="n">
-        <v>44631.51006944444</v>
-      </c>
-      <c r="BJ38" t="n">
-        <v>31.63</v>
-      </c>
-      <c r="BK38" t="n">
-        <v>0.07586537784493955</v>
-      </c>
-      <c r="BL38" t="n">
-        <v>44.94799999999999</v>
-      </c>
-      <c r="BM38" t="n">
-        <v>0.004216370213561221</v>
-      </c>
-      <c r="BN38" t="n">
-        <v>24.223</v>
-      </c>
-      <c r="BO38" t="n">
-        <v>0.0400138864784602</v>
-      </c>
-      <c r="BP38" s="2" t="n">
-        <v>44631.47489583334</v>
       </c>
     </row>
     <row r="39">
@@ -8404,7 +8288,7 @@
         <v>38</v>
       </c>
       <c r="C39" s="2" t="n">
-        <v>44631.50651620371</v>
+        <v>44631.51346064815</v>
       </c>
       <c r="D39" t="n">
         <v>2800.04075483232</v>
@@ -8568,38 +8452,35 @@
       <c r="BE39" t="n">
         <v>10</v>
       </c>
-      <c r="BF39" s="2" t="n">
+      <c r="BF39" t="n">
+        <v>2845.5</v>
+      </c>
+      <c r="BG39" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH39" s="2" t="n">
+        <v>44631.51388888889</v>
+      </c>
+      <c r="BI39" t="n">
+        <v>31.63</v>
+      </c>
+      <c r="BJ39" t="n">
+        <v>0.07586537784493955</v>
+      </c>
+      <c r="BK39" t="n">
+        <v>44.94799999999999</v>
+      </c>
+      <c r="BL39" t="n">
+        <v>0.004216370213561221</v>
+      </c>
+      <c r="BM39" t="n">
+        <v>24.223</v>
+      </c>
+      <c r="BN39" t="n">
+        <v>0.0400138864784602</v>
+      </c>
+      <c r="BO39" s="2" t="n">
         <v>44631.51346064815</v>
-      </c>
-      <c r="BG39" t="n">
-        <v>2896.5</v>
-      </c>
-      <c r="BH39" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI39" s="2" t="n">
-        <v>44631.54548611111</v>
-      </c>
-      <c r="BJ39" t="n">
-        <v>52.384</v>
-      </c>
-      <c r="BK39" t="n">
-        <v>0.009660917830792868</v>
-      </c>
-      <c r="BL39" t="n">
-        <v>44.967</v>
-      </c>
-      <c r="BM39" t="n">
-        <v>0.004830458915395017</v>
-      </c>
-      <c r="BN39" t="n">
-        <v>32.94199999999999</v>
-      </c>
-      <c r="BO39" t="n">
-        <v>0.004216370213561181</v>
-      </c>
-      <c r="BP39" s="2" t="n">
-        <v>44631.50998842593</v>
       </c>
     </row>
     <row r="40">
@@ -8610,7 +8491,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="2" t="n">
-        <v>44631.54199074074</v>
+        <v>44631.54893518519</v>
       </c>
       <c r="D40" t="n">
         <v>2851.12699390202</v>
@@ -8774,38 +8655,35 @@
       <c r="BE40" t="n">
         <v>10</v>
       </c>
-      <c r="BF40" s="2" t="n">
+      <c r="BF40" t="n">
+        <v>2896.5</v>
+      </c>
+      <c r="BG40" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH40" s="2" t="n">
+        <v>44631.54930555556</v>
+      </c>
+      <c r="BI40" t="n">
+        <v>52.384</v>
+      </c>
+      <c r="BJ40" t="n">
+        <v>0.009660917830792868</v>
+      </c>
+      <c r="BK40" t="n">
+        <v>44.967</v>
+      </c>
+      <c r="BL40" t="n">
+        <v>0.004830458915395017</v>
+      </c>
+      <c r="BM40" t="n">
+        <v>32.94199999999999</v>
+      </c>
+      <c r="BN40" t="n">
+        <v>0.004216370213561181</v>
+      </c>
+      <c r="BO40" s="2" t="n">
         <v>44631.54893518519</v>
-      </c>
-      <c r="BG40" t="n">
-        <v>2947.5</v>
-      </c>
-      <c r="BH40" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI40" s="2" t="n">
-        <v>44631.58090277778</v>
-      </c>
-      <c r="BJ40" t="n">
-        <v>73.56499999999998</v>
-      </c>
-      <c r="BK40" t="n">
-        <v>0.01957890020744733</v>
-      </c>
-      <c r="BL40" t="n">
-        <v>44.99100000000001</v>
-      </c>
-      <c r="BM40" t="n">
-        <v>0.003162277660171061</v>
-      </c>
-      <c r="BN40" t="n">
-        <v>39.16099999999999</v>
-      </c>
-      <c r="BO40" t="n">
-        <v>0.005676462121978755</v>
-      </c>
-      <c r="BP40" s="2" t="n">
-        <v>44631.54546296296</v>
       </c>
     </row>
     <row r="41">
@@ -8816,7 +8694,7 @@
         <v>40</v>
       </c>
       <c r="C41" s="2" t="n">
-        <v>44631.5775462963</v>
+        <v>44631.58449074074</v>
       </c>
       <c r="D41" t="n">
         <v>2902.31887549534</v>
@@ -8980,38 +8858,35 @@
       <c r="BE41" t="n">
         <v>10</v>
       </c>
-      <c r="BF41" s="2" t="n">
+      <c r="BF41" t="n">
+        <v>2947.5</v>
+      </c>
+      <c r="BG41" t="n">
+        <v>3.027650354097492</v>
+      </c>
+      <c r="BH41" s="2" t="n">
+        <v>44631.58472222222</v>
+      </c>
+      <c r="BI41" t="n">
+        <v>73.56499999999998</v>
+      </c>
+      <c r="BJ41" t="n">
+        <v>0.01957890020744733</v>
+      </c>
+      <c r="BK41" t="n">
+        <v>44.99100000000001</v>
+      </c>
+      <c r="BL41" t="n">
+        <v>0.003162277660171061</v>
+      </c>
+      <c r="BM41" t="n">
+        <v>39.16099999999999</v>
+      </c>
+      <c r="BN41" t="n">
+        <v>0.005676462121978755</v>
+      </c>
+      <c r="BO41" s="2" t="n">
         <v>44631.58449074074</v>
-      </c>
-      <c r="BG41" t="n">
-        <v>2999</v>
-      </c>
-      <c r="BH41" t="n">
-        <v>3.3166247903554</v>
-      </c>
-      <c r="BI41" s="2" t="n">
-        <v>44631.61666666667</v>
-      </c>
-      <c r="BJ41" t="n">
-        <v>93.13727272727273</v>
-      </c>
-      <c r="BK41" t="n">
-        <v>0.01272077756342854</v>
-      </c>
-      <c r="BL41" t="n">
-        <v>45.06181818181818</v>
-      </c>
-      <c r="BM41" t="n">
-        <v>0.004045199174782176</v>
-      </c>
-      <c r="BN41" t="n">
-        <v>43.70090909090909</v>
-      </c>
-      <c r="BO41" t="n">
-        <v>0.005393598899709359</v>
-      </c>
-      <c r="BP41" s="2" t="n">
-        <v>44631.58101851852</v>
       </c>
     </row>
     <row r="42">
@@ -9022,7 +8897,7 @@
         <v>41</v>
       </c>
       <c r="C42" s="2" t="n">
-        <v>44631.61319444444</v>
+        <v>44631.62013888889</v>
       </c>
       <c r="D42" t="n">
         <v>2953.64781356975</v>
@@ -9186,38 +9061,35 @@
       <c r="BE42" t="n">
         <v>10</v>
       </c>
-      <c r="BF42" s="2" t="n">
+      <c r="BF42" t="n">
+        <v>2999</v>
+      </c>
+      <c r="BG42" t="n">
+        <v>3.3166247903554</v>
+      </c>
+      <c r="BH42" s="2" t="n">
         <v>44631.62013888889</v>
       </c>
-      <c r="BG42" t="n">
-        <v>3050.5</v>
-      </c>
-      <c r="BH42" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BI42" s="2" t="n">
-        <v>44631.65243055556</v>
+      <c r="BI42" t="n">
+        <v>93.13727272727273</v>
       </c>
       <c r="BJ42" t="n">
-        <v>73.77700000000002</v>
+        <v>0.01272077756342854</v>
       </c>
       <c r="BK42" t="n">
-        <v>0.02584139659108227</v>
+        <v>45.06181818181818</v>
       </c>
       <c r="BL42" t="n">
-        <v>44.95199999999999</v>
+        <v>0.004045199174782176</v>
       </c>
       <c r="BM42" t="n">
-        <v>0.006324555320337483</v>
+        <v>43.70090909090909</v>
       </c>
       <c r="BN42" t="n">
-        <v>39.17300000000001</v>
-      </c>
-      <c r="BO42" t="n">
-        <v>0.008232726023485277</v>
-      </c>
-      <c r="BP42" s="2" t="n">
-        <v>44631.61666666667</v>
+        <v>0.005393598899709359</v>
+      </c>
+      <c r="BO42" s="2" t="n">
+        <v>44631.62013888889</v>
       </c>
     </row>
     <row r="43">
@@ -9228,7 +9100,7 @@
         <v>42</v>
       </c>
       <c r="C43" s="2" t="n">
-        <v>44631.64907407408</v>
+        <v>44631.65601851852</v>
       </c>
       <c r="D43" t="n">
         <v>3005.32441581785</v>
@@ -9392,9 +9264,7 @@
       <c r="BE43" t="n">
         <v>10</v>
       </c>
-      <c r="BF43" s="2" t="n">
-        <v>44631.65601851852</v>
-      </c>
+      <c r="BF43" t="inlineStr"/>
       <c r="BG43" t="inlineStr"/>
       <c r="BH43" t="inlineStr"/>
       <c r="BI43" t="inlineStr"/>
@@ -9403,9 +9273,8 @@
       <c r="BL43" t="inlineStr"/>
       <c r="BM43" t="inlineStr"/>
       <c r="BN43" t="inlineStr"/>
-      <c r="BO43" t="inlineStr"/>
-      <c r="BP43" s="2" t="n">
-        <v>44631.6525462963</v>
+      <c r="BO43" s="2" t="n">
+        <v>44631.65601851852</v>
       </c>
     </row>
     <row r="44">
@@ -9416,7 +9285,7 @@
         <v>43</v>
       </c>
       <c r="C44" s="2" t="n">
-        <v>44631.68494212963</v>
+        <v>44631.69188657407</v>
       </c>
       <c r="D44" t="n">
         <v>3056.97074382752</v>
@@ -9580,9 +9449,7 @@
       <c r="BE44" t="n">
         <v>10</v>
       </c>
-      <c r="BF44" s="2" t="n">
-        <v>44631.69188657407</v>
-      </c>
+      <c r="BF44" t="inlineStr"/>
       <c r="BG44" t="inlineStr"/>
       <c r="BH44" t="inlineStr"/>
       <c r="BI44" t="inlineStr"/>
@@ -9591,9 +9458,8 @@
       <c r="BL44" t="inlineStr"/>
       <c r="BM44" t="inlineStr"/>
       <c r="BN44" t="inlineStr"/>
-      <c r="BO44" t="inlineStr"/>
-      <c r="BP44" s="2" t="n">
-        <v>44631.68841435185</v>
+      <c r="BO44" s="2" t="n">
+        <v>44631.69188657407</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added a few calibration jobs
</commit_message>
<xml_diff>
--- a/datacombined dataloggerMSLmi70.xlsx.xlsx
+++ b/datacombined dataloggerMSLmi70.xlsx.xlsx
@@ -7336,33 +7336,15 @@
       <c r="BE34" t="n">
         <v>10</v>
       </c>
-      <c r="BF34" t="n">
-        <v>2341.5</v>
-      </c>
-      <c r="BG34" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BH34" s="2" t="n">
-        <v>44631.16388888889</v>
-      </c>
-      <c r="BI34" t="n">
-        <v>73.53999999999999</v>
-      </c>
-      <c r="BJ34" t="n">
-        <v>0.02624669291337254</v>
-      </c>
-      <c r="BK34" t="n">
-        <v>34.94499999999999</v>
-      </c>
-      <c r="BL34" t="n">
-        <v>0.005270462766950217</v>
-      </c>
-      <c r="BM34" t="n">
-        <v>29.507</v>
-      </c>
-      <c r="BN34" t="n">
-        <v>0.008232726023486557</v>
-      </c>
+      <c r="BF34" t="inlineStr"/>
+      <c r="BG34" t="inlineStr"/>
+      <c r="BH34" t="inlineStr"/>
+      <c r="BI34" t="inlineStr"/>
+      <c r="BJ34" t="inlineStr"/>
+      <c r="BK34" t="inlineStr"/>
+      <c r="BL34" t="inlineStr"/>
+      <c r="BM34" t="inlineStr"/>
+      <c r="BN34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -7536,33 +7518,15 @@
       <c r="BE35" t="n">
         <v>10</v>
       </c>
-      <c r="BF35" t="n">
-        <v>2392.5</v>
-      </c>
-      <c r="BG35" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BH35" s="2" t="n">
-        <v>44631.19930555556</v>
-      </c>
-      <c r="BI35" t="n">
-        <v>52.496</v>
-      </c>
-      <c r="BJ35" t="n">
-        <v>0.01074967699773214</v>
-      </c>
-      <c r="BK35" t="n">
-        <v>34.941</v>
-      </c>
-      <c r="BL35" t="n">
-        <v>0.0031622776601692</v>
-      </c>
-      <c r="BM35" t="n">
-        <v>23.777</v>
-      </c>
-      <c r="BN35" t="n">
-        <v>0.004830458915398123</v>
-      </c>
+      <c r="BF35" t="inlineStr"/>
+      <c r="BG35" t="inlineStr"/>
+      <c r="BH35" t="inlineStr"/>
+      <c r="BI35" t="inlineStr"/>
+      <c r="BJ35" t="inlineStr"/>
+      <c r="BK35" t="inlineStr"/>
+      <c r="BL35" t="inlineStr"/>
+      <c r="BM35" t="inlineStr"/>
+      <c r="BN35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -7736,33 +7700,15 @@
       <c r="BE36" t="n">
         <v>10</v>
       </c>
-      <c r="BF36" t="n">
-        <v>2443.5</v>
-      </c>
-      <c r="BG36" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BH36" s="2" t="n">
-        <v>44631.23472222222</v>
-      </c>
-      <c r="BI36" t="n">
-        <v>31.712</v>
-      </c>
-      <c r="BJ36" t="n">
-        <v>0.02616188916046516</v>
-      </c>
-      <c r="BK36" t="n">
-        <v>34.94</v>
-      </c>
-      <c r="BL36" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM36" t="n">
-        <v>15.645</v>
-      </c>
-      <c r="BN36" t="n">
-        <v>0.01354006400772616</v>
-      </c>
+      <c r="BF36" t="inlineStr"/>
+      <c r="BG36" t="inlineStr"/>
+      <c r="BH36" t="inlineStr"/>
+      <c r="BI36" t="inlineStr"/>
+      <c r="BJ36" t="inlineStr"/>
+      <c r="BK36" t="inlineStr"/>
+      <c r="BL36" t="inlineStr"/>
+      <c r="BM36" t="inlineStr"/>
+      <c r="BN36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -7936,33 +7882,15 @@
       <c r="BE37" t="n">
         <v>10</v>
       </c>
-      <c r="BF37" t="n">
-        <v>2493.5</v>
-      </c>
-      <c r="BG37" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BH37" s="2" t="n">
-        <v>44631.26944444444</v>
-      </c>
-      <c r="BI37" t="n">
-        <v>10.269</v>
-      </c>
-      <c r="BJ37" t="n">
-        <v>0.007378647873725878</v>
-      </c>
-      <c r="BK37" t="n">
-        <v>34.94</v>
-      </c>
-      <c r="BL37" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM37" t="n">
-        <v>-0.7370000000000001</v>
-      </c>
-      <c r="BN37" t="n">
-        <v>0.009486832980505148</v>
-      </c>
+      <c r="BF37" t="inlineStr"/>
+      <c r="BG37" t="inlineStr"/>
+      <c r="BH37" t="inlineStr"/>
+      <c r="BI37" t="inlineStr"/>
+      <c r="BJ37" t="inlineStr"/>
+      <c r="BK37" t="inlineStr"/>
+      <c r="BL37" t="inlineStr"/>
+      <c r="BM37" t="inlineStr"/>
+      <c r="BN37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -8136,33 +8064,15 @@
       <c r="BE38" t="n">
         <v>10</v>
       </c>
-      <c r="BF38" t="n">
-        <v>2794.5</v>
-      </c>
-      <c r="BG38" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BH38" s="2" t="n">
-        <v>44631.47847222222</v>
-      </c>
-      <c r="BI38" t="n">
-        <v>10.145</v>
-      </c>
-      <c r="BJ38" t="n">
-        <v>0.005270462766947264</v>
-      </c>
-      <c r="BK38" t="n">
-        <v>44.93</v>
-      </c>
-      <c r="BL38" t="n">
-        <v>0</v>
-      </c>
-      <c r="BM38" t="n">
-        <v>6.51</v>
-      </c>
-      <c r="BN38" t="n">
-        <v>0.006666666666666251</v>
-      </c>
+      <c r="BF38" t="inlineStr"/>
+      <c r="BG38" t="inlineStr"/>
+      <c r="BH38" t="inlineStr"/>
+      <c r="BI38" t="inlineStr"/>
+      <c r="BJ38" t="inlineStr"/>
+      <c r="BK38" t="inlineStr"/>
+      <c r="BL38" t="inlineStr"/>
+      <c r="BM38" t="inlineStr"/>
+      <c r="BN38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -8336,33 +8246,15 @@
       <c r="BE39" t="n">
         <v>10</v>
       </c>
-      <c r="BF39" t="n">
-        <v>2845.5</v>
-      </c>
-      <c r="BG39" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BH39" s="2" t="n">
-        <v>44631.51388888889</v>
-      </c>
-      <c r="BI39" t="n">
-        <v>31.63</v>
-      </c>
-      <c r="BJ39" t="n">
-        <v>0.07586537784493955</v>
-      </c>
-      <c r="BK39" t="n">
-        <v>44.94799999999999</v>
-      </c>
-      <c r="BL39" t="n">
-        <v>0.004216370213561221</v>
-      </c>
-      <c r="BM39" t="n">
-        <v>24.223</v>
-      </c>
-      <c r="BN39" t="n">
-        <v>0.0400138864784602</v>
-      </c>
+      <c r="BF39" t="inlineStr"/>
+      <c r="BG39" t="inlineStr"/>
+      <c r="BH39" t="inlineStr"/>
+      <c r="BI39" t="inlineStr"/>
+      <c r="BJ39" t="inlineStr"/>
+      <c r="BK39" t="inlineStr"/>
+      <c r="BL39" t="inlineStr"/>
+      <c r="BM39" t="inlineStr"/>
+      <c r="BN39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -8536,33 +8428,15 @@
       <c r="BE40" t="n">
         <v>10</v>
       </c>
-      <c r="BF40" t="n">
-        <v>2896.5</v>
-      </c>
-      <c r="BG40" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BH40" s="2" t="n">
-        <v>44631.54930555556</v>
-      </c>
-      <c r="BI40" t="n">
-        <v>52.384</v>
-      </c>
-      <c r="BJ40" t="n">
-        <v>0.009660917830792868</v>
-      </c>
-      <c r="BK40" t="n">
-        <v>44.967</v>
-      </c>
-      <c r="BL40" t="n">
-        <v>0.004830458915395017</v>
-      </c>
-      <c r="BM40" t="n">
-        <v>32.94199999999999</v>
-      </c>
-      <c r="BN40" t="n">
-        <v>0.004216370213561181</v>
-      </c>
+      <c r="BF40" t="inlineStr"/>
+      <c r="BG40" t="inlineStr"/>
+      <c r="BH40" t="inlineStr"/>
+      <c r="BI40" t="inlineStr"/>
+      <c r="BJ40" t="inlineStr"/>
+      <c r="BK40" t="inlineStr"/>
+      <c r="BL40" t="inlineStr"/>
+      <c r="BM40" t="inlineStr"/>
+      <c r="BN40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -8736,33 +8610,15 @@
       <c r="BE41" t="n">
         <v>10</v>
       </c>
-      <c r="BF41" t="n">
-        <v>2947.5</v>
-      </c>
-      <c r="BG41" t="n">
-        <v>3.027650354097492</v>
-      </c>
-      <c r="BH41" s="2" t="n">
-        <v>44631.58472222222</v>
-      </c>
-      <c r="BI41" t="n">
-        <v>73.56499999999998</v>
-      </c>
-      <c r="BJ41" t="n">
-        <v>0.01957890020744733</v>
-      </c>
-      <c r="BK41" t="n">
-        <v>44.99100000000001</v>
-      </c>
-      <c r="BL41" t="n">
-        <v>0.003162277660171061</v>
-      </c>
-      <c r="BM41" t="n">
-        <v>39.16099999999999</v>
-      </c>
-      <c r="BN41" t="n">
-        <v>0.005676462121978755</v>
-      </c>
+      <c r="BF41" t="inlineStr"/>
+      <c r="BG41" t="inlineStr"/>
+      <c r="BH41" t="inlineStr"/>
+      <c r="BI41" t="inlineStr"/>
+      <c r="BJ41" t="inlineStr"/>
+      <c r="BK41" t="inlineStr"/>
+      <c r="BL41" t="inlineStr"/>
+      <c r="BM41" t="inlineStr"/>
+      <c r="BN41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -8936,33 +8792,15 @@
       <c r="BE42" t="n">
         <v>10</v>
       </c>
-      <c r="BF42" t="n">
-        <v>2999</v>
-      </c>
-      <c r="BG42" t="n">
-        <v>3.3166247903554</v>
-      </c>
-      <c r="BH42" s="2" t="n">
-        <v>44631.62013888889</v>
-      </c>
-      <c r="BI42" t="n">
-        <v>93.13727272727273</v>
-      </c>
-      <c r="BJ42" t="n">
-        <v>0.01272077756342854</v>
-      </c>
-      <c r="BK42" t="n">
-        <v>45.06181818181818</v>
-      </c>
-      <c r="BL42" t="n">
-        <v>0.004045199174782176</v>
-      </c>
-      <c r="BM42" t="n">
-        <v>43.70090909090909</v>
-      </c>
-      <c r="BN42" t="n">
-        <v>0.005393598899709359</v>
-      </c>
+      <c r="BF42" t="inlineStr"/>
+      <c r="BG42" t="inlineStr"/>
+      <c r="BH42" t="inlineStr"/>
+      <c r="BI42" t="inlineStr"/>
+      <c r="BJ42" t="inlineStr"/>
+      <c r="BK42" t="inlineStr"/>
+      <c r="BL42" t="inlineStr"/>
+      <c r="BM42" t="inlineStr"/>
+      <c r="BN42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">

</xml_diff>